<commit_message>
đôi font-end mới và thêm pdf
</commit_message>
<xml_diff>
--- a/Admin/KhenThuong_output.xlsx
+++ b/Admin/KhenThuong_output.xlsx
@@ -15,7 +15,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+  <si>
+    <t>STT</t>
+  </si>
   <si>
     <t>Đơn Vị</t>
   </si>
@@ -432,26 +435,27 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A2" sqref="A2:I10"/>
+      <selection activeCell="A2" sqref="A2:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="25.708" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="8.141" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="33.992" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="32.849" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="28.136" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="44.703" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="37.562" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="36.42" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="37.562" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="6.856" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="25.708" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="8.141" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="33.992" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="32.849" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="28.136" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="44.703" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="37.562" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="36.42" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="37.562" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -479,159 +483,189 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2">
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2">
         <v>2024</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2">
         <v>2024</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2">
         <v>2024</v>
       </c>
-      <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2">
         <v>2024</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2">
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2">
         <v>2024</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="2">
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2">
         <v>2024</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="2">
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="2">
         <v>2022</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="2">
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2">
         <v>2022</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="2" t="s">
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="2">
         <v>2021</v>
       </c>
-      <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" s="2"/>
     </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>

</xml_diff>

<commit_message>
thêm sửa tài khoản cho trang tài khoản
</commit_message>
<xml_diff>
--- a/Admin/KhenThuong_output.xlsx
+++ b/Admin/KhenThuong_output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
   <si>
     <t>STT</t>
   </si>
@@ -47,19 +47,43 @@
     <t>Huân Chương Lao Động Hạng Nhì</t>
   </si>
   <si>
-    <t>Công Nghệ Thông Tin</t>
+    <t>Khoa Nông nghiệp</t>
   </si>
   <si>
     <t>X</t>
   </si>
   <si>
-    <t>Ngoại Ngữ</t>
-  </si>
-  <si>
-    <t>Xây Dựng</t>
-  </si>
-  <si>
-    <t>Kinh Tế</t>
+    <t>Phòng Kế hoạch - Tài chính</t>
+  </si>
+  <si>
+    <t>Phòng Quản lý đào tạo</t>
+  </si>
+  <si>
+    <t>Phòng Quản lý Khoa học - Hợp tác</t>
+  </si>
+  <si>
+    <t>Trung tâm Kỹ thuật -Nông nghiệp</t>
+  </si>
+  <si>
+    <t>Trung tâm Ngoại ngữ - Tin học</t>
+  </si>
+  <si>
+    <t>2021-2022</t>
+  </si>
+  <si>
+    <t>2022-2023</t>
+  </si>
+  <si>
+    <t>Khoa Công nghệ - Thủy sản</t>
+  </si>
+  <si>
+    <t>2023-2024</t>
+  </si>
+  <si>
+    <t>Khoa Công nghệ thông tin - Truyền thông</t>
+  </si>
+  <si>
+    <t>2024-2025</t>
   </si>
 </sst>
 </file>
@@ -435,17 +459,17 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A2" sqref="A2:J10"/>
+      <selection activeCell="A2" sqref="A2:J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="6.856" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="25.708" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="8.141" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="49.417" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="13.997" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="33.992" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="32.849" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="28.136" bestFit="true" customWidth="true" style="0"/>
@@ -495,12 +519,12 @@
         <v>10</v>
       </c>
       <c r="C2" s="2">
-        <v>2024</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
-        <v>11</v>
-      </c>
+        <v>2015</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -512,10 +536,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2">
-        <v>2024</v>
+        <v>2017</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
@@ -532,16 +556,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2">
-        <v>2024</v>
+        <v>2017</v>
       </c>
       <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -555,14 +579,14 @@
         <v>12</v>
       </c>
       <c r="C5" s="2">
-        <v>2024</v>
+        <v>2017</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -575,14 +599,14 @@
         <v>13</v>
       </c>
       <c r="C6" s="2">
-        <v>2024</v>
+        <v>2017</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -595,14 +619,14 @@
         <v>14</v>
       </c>
       <c r="C7" s="2">
-        <v>2024</v>
+        <v>2017</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -612,15 +636,15 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8" s="2">
-        <v>2022</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="2"/>
+        <v>2019</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -632,15 +656,15 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="2">
-        <v>2022</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="2"/>
+        <v>2019</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
@@ -652,20 +676,200 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C10" s="2">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="I10" s="2"/>
       <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" s="2"/>
     </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>

</xml_diff>